<commit_message>
updated on Oct 9
</commit_message>
<xml_diff>
--- a/result-all.xlsx
+++ b/result-all.xlsx
@@ -5,19 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Desktop/JULIA-ENERGISE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116B31DF-B12A-4945-A8D3-CC5830000322}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B3F4F07-B822-024F-8F8B-E660773AD058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12800" yWindow="460" windowWidth="12800" windowHeight="15540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Solar" sheetId="5" r:id="rId1"/>
     <sheet name="Cost" sheetId="4" r:id="rId2"/>
-    <sheet name="result.csv" sheetId="1" r:id="rId3"/>
-    <sheet name="MAx" sheetId="2" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId5"/>
+    <sheet name="Battery" sheetId="6" r:id="rId3"/>
+    <sheet name="result.csv" sheetId="1" r:id="rId4"/>
+    <sheet name="MAx" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="11">
   <si>
     <t>PredLength</t>
   </si>
@@ -68,6 +69,9 @@
   </si>
   <si>
     <t>Pg</t>
+  </si>
+  <si>
+    <t>detministic setup</t>
   </si>
 </sst>
 </file>
@@ -109,9 +113,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="173" zoomScaleNormal="200" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="173" zoomScaleNormal="200" workbookViewId="0">
       <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
@@ -713,10 +727,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E36"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+    <sheetView topLeftCell="A19" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1054,22 +1068,356 @@
         <v>8123.33</v>
       </c>
     </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>23700.11</v>
+      </c>
+      <c r="C34">
+        <v>16002.47</v>
+      </c>
+      <c r="D34">
+        <v>10752.28</v>
+      </c>
+      <c r="E34">
+        <v>8121.33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>15</v>
+      </c>
+      <c r="B35">
+        <v>22459.47</v>
+      </c>
+      <c r="C35">
+        <v>14685.72</v>
+      </c>
+      <c r="D35">
+        <v>9092.3700000000008</v>
+      </c>
+      <c r="E35">
+        <v>6094.08</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>20912.47</v>
+      </c>
+      <c r="C36">
+        <v>13101.62</v>
+      </c>
+      <c r="D36">
+        <v>7160.02</v>
+      </c>
+      <c r="E36">
+        <v>3750.06</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D03F280F-F24D-E14D-8242-94BF5578569C}">
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="A1:E29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="2">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2">
+        <v>24025.820426014223</v>
+      </c>
+      <c r="C2" s="2">
+        <v>17860.145015957976</v>
+      </c>
+      <c r="D2" s="2">
+        <v>11190.917434693136</v>
+      </c>
+      <c r="E2" s="2">
+        <v>8615.2970136409349</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2">
+        <v>23505.235062796452</v>
+      </c>
+      <c r="C3" s="2">
+        <v>17339.559809490325</v>
+      </c>
+      <c r="D3" s="2">
+        <v>10657.0707664399</v>
+      </c>
+      <c r="E3" s="2">
+        <v>8002.8492457905486</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2">
+        <v>22851.462678712902</v>
+      </c>
+      <c r="C4" s="2">
+        <v>16685.787744748824</v>
+      </c>
+      <c r="D4" s="2">
+        <v>10016.551889938706</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7283.7349684510646</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>3</v>
+      </c>
+      <c r="B9" s="3">
+        <v>23700.11</v>
+      </c>
+      <c r="C9" s="3">
+        <v>16002.47</v>
+      </c>
+      <c r="D9" s="3">
+        <v>10752.28</v>
+      </c>
+      <c r="E9" s="3">
+        <v>8121.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
+        <v>15</v>
+      </c>
+      <c r="B10" s="3">
+        <v>22459.47</v>
+      </c>
+      <c r="C10" s="3">
+        <v>14685.72</v>
+      </c>
+      <c r="D10" s="3">
+        <v>9092.3700000000008</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6094.08</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
+        <v>20912.47</v>
+      </c>
+      <c r="C11" s="3">
+        <v>13101.62</v>
+      </c>
+      <c r="D11" s="3">
+        <v>7160.02</v>
+      </c>
+      <c r="E11" s="3">
+        <v>3750.06</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>3</v>
+      </c>
+      <c r="B17" s="5">
+        <f>(B2-B9)/B9</f>
+        <v>1.3742992163927607E-2</v>
+      </c>
+      <c r="C17" s="5">
+        <f>(C2-C9)/C9</f>
+        <v>0.1160867676026249</v>
+      </c>
+      <c r="D17" s="5">
+        <f>(D2-D9)/D9</f>
+        <v>4.0794829998208305E-2</v>
+      </c>
+      <c r="E17" s="5">
+        <f>(E2-E9)/E9</f>
+        <v>6.0823413608477303E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>15</v>
+      </c>
+      <c r="B18" s="5">
+        <f>(B3-B10)/B10</f>
+        <v>4.6562321497188058E-2</v>
+      </c>
+      <c r="C18" s="5">
+        <f>(C3-C10)/C10</f>
+        <v>0.1807088661291599</v>
+      </c>
+      <c r="D18" s="5">
+        <f>(D3-D10)/D10</f>
+        <v>0.17208942953706224</v>
+      </c>
+      <c r="E18" s="5">
+        <f>(E3-E10)/E10</f>
+        <v>0.313216965610978</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>30</v>
+      </c>
+      <c r="B19" s="5">
+        <f>(B4-B11)/B11</f>
+        <v>9.2719448191098452E-2</v>
+      </c>
+      <c r="C19" s="5">
+        <f>(C4-C11)/C11</f>
+        <v>0.27356676080887887</v>
+      </c>
+      <c r="D19" s="5">
+        <f>(D4-D11)/D11</f>
+        <v>0.39895585346670898</v>
+      </c>
+      <c r="E19" s="5">
+        <f>(E4-E11)/E11</f>
+        <v>0.94229824814831353</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:B7"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E35"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:E35"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1339,6 +1687,73 @@
       </c>
       <c r="E29">
         <v>2888.4498440366401</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>3</v>
+      </c>
+      <c r="E32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>23700.11</v>
+      </c>
+      <c r="C33">
+        <v>16002.47</v>
+      </c>
+      <c r="D33">
+        <v>10752.28</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>15</v>
+      </c>
+      <c r="B34">
+        <v>22459.47</v>
+      </c>
+      <c r="C34">
+        <v>14685.72</v>
+      </c>
+      <c r="D34">
+        <v>9092.3700000000008</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>30</v>
+      </c>
+      <c r="B35">
+        <v>20912.47</v>
+      </c>
+      <c r="C35">
+        <v>13101.62</v>
+      </c>
+      <c r="D35">
+        <v>7160.02</v>
+      </c>
+      <c r="E35">
+        <v>3750.06</v>
       </c>
     </row>
   </sheetData>
@@ -1346,7 +1761,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I29"/>
   <sheetViews>
@@ -1825,7 +2240,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:J32"/>
   <sheetViews>

</xml_diff>